<commit_message>
Finalizado etapas de criação de executável
</commit_message>
<xml_diff>
--- a/arquivos/lista_entidades.xlsx
+++ b/arquivos/lista_entidades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prog-1\Documents\PROJETOS\py_Verificar_Precatórios\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prog-1\Documents\PROJETOS\py_Verificar_Precatórios\arquivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5713BB69-F99A-4AF2-83AC-1B0624016EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D11165-4C5B-4493-999E-B0297ED69AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="811">
   <si>
     <t>AMERIPREV - INST. DE PREV. SOC. DOS SERV. MUN. DE AMERICANA</t>
   </si>
@@ -2852,7 +2852,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C17"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2879,9 +2879,6 @@
       <c r="B2" s="3" t="s">
         <v>665</v>
       </c>
-      <c r="C2" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -2890,9 +2887,6 @@
       <c r="B3" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C3" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2901,9 +2895,6 @@
       <c r="B4" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C4" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -2912,9 +2903,6 @@
       <c r="B5" t="s">
         <v>727</v>
       </c>
-      <c r="C5" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -2923,9 +2911,6 @@
       <c r="B6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -2934,9 +2919,6 @@
       <c r="B7" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2945,9 +2927,6 @@
       <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2956,9 +2935,6 @@
       <c r="B9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -2967,9 +2943,6 @@
       <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="C10" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2978,9 +2951,6 @@
       <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2989,9 +2959,6 @@
       <c r="B12" t="s">
         <v>66</v>
       </c>
-      <c r="C12" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -3000,9 +2967,6 @@
       <c r="B13" t="s">
         <v>67</v>
       </c>
-      <c r="C13" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -3022,9 +2986,6 @@
       <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="C15" t="s">
-        <v>808</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -3033,22 +2994,16 @@
       <c r="B16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>983</v>
       </c>
       <c r="B17" t="s">
         <v>71</v>
       </c>
-      <c r="C17" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1424</v>
       </c>
@@ -3056,7 +3011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>851</v>
       </c>
@@ -3064,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>949</v>
       </c>
@@ -3072,7 +3027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1261</v>
       </c>
@@ -3080,7 +3035,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1063</v>
       </c>
@@ -3088,7 +3043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>959</v>
       </c>
@@ -3096,7 +3051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1406</v>
       </c>
@@ -3104,7 +3059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1441</v>
       </c>
@@ -3112,7 +3067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>49</v>
       </c>
@@ -3120,7 +3075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>50</v>
       </c>
@@ -3128,7 +3083,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>798</v>
       </c>
@@ -3136,7 +3091,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>36</v>
       </c>
@@ -3144,7 +3099,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1113</v>
       </c>
@@ -3152,7 +3107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1215</v>
       </c>
@@ -3160,7 +3115,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1081</v>
       </c>

</xml_diff>